<commit_message>
Combine sub-circuits, update BOM/lib, add PDFs
</commit_message>
<xml_diff>
--- a/Electrical/BOM.xlsx
+++ b/Electrical/BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t>GotT Translation Circuit BOM</t>
   </si>
@@ -98,6 +98,63 @@
     <t>http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/FOD817D3SD/?qs=32VJUWvZ7XaI9Lc6ol43XQ==</t>
   </si>
   <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>AP7313-18SAG-7</t>
+  </si>
+  <si>
+    <t>1.8V, 150mA LDO Regulator</t>
+  </si>
+  <si>
+    <t>http://www.diodes.com/_files/datasheets/AP7313.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/diodes-incorporated/AP7313-18SAG-7/AP7313-18SAG-7DICT-ND/2270838</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Diodes-Incorporated/AP7313-18SAG-7/?qs=/ha2pyFadujy/gnw%2B3xItPhBQ0SnhtM987cdGDCE3x6s1BRWXYc%2B1Q==</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>W25Q128FVSIG</t>
+  </si>
+  <si>
+    <t>Winbond 128Mb SPI NOR Flash</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128fv_revhh1_100913_website1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-search/en/integrated-circuits-ics/memory/2556980?k=w25q128fv&amp;k=&amp;pkeyword=w25q128fv&amp;pv16=7409&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>WT32i-E-AI6</t>
+  </si>
+  <si>
+    <t>WT32i BT Module, U.FL Antenna</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/368/Bluegigga%20Technologies_WT32i_Datasheet-558681.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/silicon-labs/WT32I-E-AI6/1446-1037-1-ND/4806564</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Silicon-Labs-Bluegiga/WT32i-E-AI6/?qs=sGAEpiMZZMs8jstQXqv0yeC3dKQ4sq/l%2BU8bwDMPAJ4=</t>
+  </si>
+  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -173,10 +230,28 @@
     <t>D3</t>
   </si>
   <si>
+    <t>LG L29K-G2J1-24-Z</t>
+  </si>
+  <si>
+    <t>PWR LED (Green)</t>
+  </si>
+  <si>
+    <t>http://www.osram-os.com/Graphics/XPic2/00077107_0.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-L29K-G2J1-24-Z/475-2709-1-ND/1938876</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Osram-Opto-Semiconductor/LG-L29K-G2J1-24-Z/?qs=/ha2pyFadujpFotHoYnHK8u84Sh%2BBbQboBL3gK2afekn5czm8naaMg==</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
     <t>LB Q39G-L2OO-35-1</t>
   </si>
   <si>
-    <t>PWR LED (Blue)</t>
+    <t>CONN LED (Blue)</t>
   </si>
   <si>
     <t>https://media.digikey.com/pdf/Data Sheets/Osram PDFs/LB_LT Q39G.pdf</t>
@@ -206,13 +281,31 @@
     <t>http://www.mouser.com/ProductDetail/Ohmite/OK1045E-R52/?qs=sGAEpiMZZMsPqMdJzcrNwhqiT%2B35FJji0CucJiszflQ=</t>
   </si>
   <si>
-    <t>R2, 3</t>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF8200V</t>
+  </si>
+  <si>
+    <t>PWR LED Resistor (820 Ohm), 0603</t>
+  </si>
+  <si>
+    <t>http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF8200V+7+WW</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF8200V/P820HCT-ND/1746806</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF8200V/?qs=/ha2pyFaduglTbPDDZSypYYGUgtAbfv2yF2HHUYX9QFp3giBobQZgg==</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
   <si>
     <t>ERJ-3EKF1000V</t>
   </si>
   <si>
-    <t>PWR LED Resistor, 100 Ohm, 0603</t>
+    <t>MOSFET Gate Current Limit Resistor, 100 Ohm</t>
   </si>
   <si>
     <t>http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW</t>
@@ -221,16 +314,16 @@
     <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1000V/P100HCT-ND/198109</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=/ha2pyFaduglTbPDDZSypXi%2B1JYi5TJRT2R7dib9ms/8H45gLlep/g==</t>
-  </si>
-  <si>
-    <t>R4</t>
+    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=H7k1u0Mp9JS7i8KGO5m47A==</t>
+  </si>
+  <si>
+    <t>R4, 7, 8</t>
   </si>
   <si>
     <t>ERJ-3EKF1002V</t>
   </si>
   <si>
-    <t>MOSFET Gate Pull-down Resistor, 10K Ohm</t>
+    <t>Pull-up/Pull-down Resistors, 10K Ohm</t>
   </si>
   <si>
     <t>http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1002V+7+WW</t>
@@ -260,6 +353,9 @@
     <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF2200V/?qs=iBwFsHVUAOcTUCNoJPNpnQ==</t>
   </si>
   <si>
+    <t>R6</t>
+  </si>
+  <si>
     <t>F1</t>
   </si>
   <si>
@@ -314,7 +410,22 @@
     <t>http://www.mouser.com/ProductDetail/AVX/TPSD107K016R0125/?qs=Ow%2BOiPmaljGaFh%2BHI/q%2BNg==</t>
   </si>
   <si>
-    <t>C3</t>
+    <t>C3, 6</t>
+  </si>
+  <si>
+    <t>0.1uF Filter Capacitors</t>
+  </si>
+  <si>
+    <t>C4, 5</t>
+  </si>
+  <si>
+    <t>2.2uF Filter Capacitors</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>0.15uF Analog Filter Capacitor</t>
   </si>
   <si>
     <t>L1</t>
@@ -335,6 +446,24 @@
     <t>http://www.mouser.com/ProductDetail/Pulse/PE-53820SNL/?qs=sGAEpiMZZMsg%2By3WlYCkU6/kcGZFUWykAerZ435ceU4=</t>
   </si>
   <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>MPZ1608S601ATA00</t>
+  </si>
+  <si>
+    <t>Ferrite Bead 600 Ohm at 100MHz</t>
+  </si>
+  <si>
+    <t>https://product.tdk.com/info/en/catalog/datasheets/beads_commercial_power_mpz1608_en.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tdk-corporation/MPZ1608S601ATA00/445-2205-1-ND/765103</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TDK/MPZ1608S601ATA00/?qs=47dIwT2ZIzth0CTKDYh9rw==</t>
+  </si>
+  <si>
     <t>SW1</t>
   </si>
   <si>
@@ -356,6 +485,9 @@
     <t>P1</t>
   </si>
   <si>
+    <t>P2</t>
+  </si>
+  <si>
     <t>Lights Screw Terminal, 01X03</t>
   </si>
   <si>
@@ -368,7 +500,7 @@
     <t>http://www.mouser.com/ProductDetail/Phoenix-Contact/1935174/?qs=QWULklcAmSR8B7o4YouITA==</t>
   </si>
   <si>
-    <t>P2</t>
+    <t>P3</t>
   </si>
   <si>
     <t>68000-103HLF</t>
@@ -384,6 +516,45 @@
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/FCI/68000-103HLF/?qs=zh4O8xspOuyqPBhcuxtliw==</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>PGT1</t>
+  </si>
+  <si>
+    <t>JF1R6-CR3-4I</t>
+  </si>
+  <si>
+    <t>U.FL (UMCC) to RP-SMA Female</t>
+  </si>
+  <si>
+    <t>http://www.digi.com/products/models/jf1r6-cr3-4i</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/digi-international/JF1R6-CR3-4I/JF1R6-CR3-4I-ND/1090366</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Digi-International/JF1R6-CR3-4I/?qs=/ha2pyFaduims8tK6Us52r5eWOHgAet92us06mmlXyAvpYrNpBxg1A==</t>
+  </si>
+  <si>
+    <t>ANT1</t>
+  </si>
+  <si>
+    <t>001-0015</t>
+  </si>
+  <si>
+    <t>2.4 GHz u.FL Antenna</t>
+  </si>
+  <si>
+    <t>http://www.lsr.com/downloads/products/330-0150.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lsr/001-0015/001-0015-ND/4732759</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/LS-Research/001-0015/?qs=sGAEpiMZZMuBTKBKvsBmlP%2BmDojcpAG/Vyhv39d/eWhHn2QU78Oagg==</t>
   </si>
   <si>
     <t>Cost/Board:</t>
@@ -548,12 +719,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -579,24 +750,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMI30"/>
+  <dimension ref="1:39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="33.9030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="37.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.61224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.1734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.9183673469388"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.9591836734694"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.280612244898"/>
     <col collapsed="false" hidden="false" max="1021" min="11" style="1" width="11.5204081632653"/>
@@ -2716,6 +2886,8 @@
       <c r="H4" s="10" t="s">
         <v>20</v>
       </c>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -2742,6 +2914,8 @@
       <c r="H5" s="10" t="s">
         <v>26</v>
       </c>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -2751,7 +2925,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>2.25</v>
+        <v>0.41</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>28</v>
@@ -2768,286 +2942,256 @@
       <c r="H6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="0"/>
-      <c r="L6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>0.24</v>
+        <v>1.61</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="0"/>
-      <c r="L8" s="0"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>50</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="5" customFormat="true" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="7" t="n">
-        <v>0.35</v>
+        <v>19.66</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="K10" s="0"/>
-      <c r="L10" s="0"/>
+        <v>45</v>
+      </c>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+      <c r="AMH10" s="0"/>
+      <c r="AMI10" s="0"/>
+      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>0.1</v>
+        <v>2.25</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="10"/>
+        <v>51</v>
+      </c>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>64</v>
+        <v>0.88</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="10"/>
+        <v>57</v>
+      </c>
       <c r="K12" s="0"/>
       <c r="L12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="7" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>70</v>
+        <v>0.24</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K13" s="0"/>
       <c r="L13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>0.1</v>
+        <v>0.44</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>80</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="7" t="n">
-        <v>0.18</v>
+        <v>0.37</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>85</v>
+        <v>73</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>86</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="I15" s="10"/>
       <c r="K15" s="0"/>
       <c r="L15" s="0"/>
+      <c r="AMH15" s="1"/>
+      <c r="AMI15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="7" t="n">
-        <v>0.89</v>
+        <v>0.35</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="I16" s="10"/>
       <c r="K16" s="0"/>
@@ -3057,48 +3201,58 @@
     </row>
     <row r="17" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="7" t="n">
-        <v>1.39</v>
+        <v>0.1</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="I17" s="10"/>
       <c r="K17" s="0"/>
       <c r="L17" s="0"/>
-      <c r="AMH17" s="1"/>
-      <c r="AMI17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
+      <c r="C18" s="7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="I18" s="10"/>
       <c r="K18" s="0"/>
       <c r="L18" s="0"/>
@@ -3107,190 +3261,493 @@
     </row>
     <row r="19" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="7" t="n">
-        <v>3.24</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>101</v>
+        <v>0.1</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="I19" s="10"/>
-      <c r="K19" s="0"/>
-      <c r="L19" s="0"/>
-      <c r="AMH19" s="1"/>
-      <c r="AMI19" s="1"/>
+        <v>99</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B20" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" s="7" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>107</v>
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="I20" s="10"/>
+        <v>105</v>
+      </c>
       <c r="K20" s="0"/>
       <c r="L20" s="0"/>
-      <c r="AMH20" s="1"/>
-      <c r="AMI20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="7" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="D21" s="11" t="n">
-        <v>1935174</v>
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>116</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>122</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="A23" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="A24" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" s="10"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="0"/>
+      <c r="AMH24" s="1"/>
+      <c r="AMI24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="A25" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="AMH25" s="1"/>
+      <c r="AMI25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>2</v>
+      </c>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>132</v>
+      </c>
       <c r="F26" s="9"/>
-      <c r="G26" s="10"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+      <c r="AMH26" s="1"/>
+      <c r="AMI26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="6" t="n">
+        <v>2</v>
+      </c>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="F27" s="9"/>
-      <c r="G27" s="10"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+      <c r="AMH27" s="1"/>
+      <c r="AMI27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="F28" s="9"/>
-      <c r="G28" s="10"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="AMH28" s="1"/>
+      <c r="AMI28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="13"/>
-      <c r="C29" s="7"/>
-      <c r="G29" s="0"/>
+      <c r="A29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I29" s="10"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+      <c r="AMH29" s="1"/>
+      <c r="AMI29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14" t="s">
-        <v>123</v>
+      <c r="A30" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="C30" s="7" t="n">
-        <f aca="false">(C6*B6)+(C8*B8)+(C9*B9)+(C11*B11)+(C12*B12)+(C15*B15)+(C16*B16)+(C17*B17)+(C19*B19)+(C24*B24)+(C26*B26)+(C28*B28)</f>
-        <v>8.93</v>
-      </c>
-      <c r="G30" s="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="I31" s="10"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="AMH31" s="1"/>
+      <c r="AMI31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="AMH32" s="1"/>
+      <c r="AMI32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="D33" s="12" t="n">
+        <v>1935174</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B34" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I37" s="10"/>
+      <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
+      <c r="AMH37" s="1"/>
+      <c r="AMI37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="13"/>
+      <c r="C38" s="7"/>
+      <c r="G38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="7" t="n">
+        <f aca="false">(C11*B11)+(C13*B13)+(C14*B14)+(C17*B17)+(C18*B18)+(C23*B23)+(C24*B24)+(C25*B25)+(C29*B29)+(C29*B29)+(C33*B33)+(C35*B35)</f>
+        <v>12.6</v>
+      </c>
+      <c r="G39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3306,58 +3763,81 @@
     <hyperlink ref="F5" r:id="rId7" display="https://www.fairchildsemi.com/datasheets/FO/FOD817D.pdf"/>
     <hyperlink ref="G5" r:id="rId8" display="https://www.digikey.com/product-detail/en/fairchild-semiconductor/FOD817D3SD/FOD817D3SDCT-ND/3041737"/>
     <hyperlink ref="H5" r:id="rId9" display="http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/FOD817D3SD/?qs=32VJUWvZ7XaI9Lc6ol43XQ=="/>
-    <hyperlink ref="F6" r:id="rId10" display="https://www.fairchildsemi.com/datasheets/FQ/FQP47P06.pdf"/>
-    <hyperlink ref="G6" r:id="rId11" display="https://www.digikey.com/product-detail/en/fairchild-semiconductor/FQP47P06/FQP47P06-ND/1057079"/>
-    <hyperlink ref="H6" r:id="rId12" display="http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/FQP47P06/?qs=/ha2pyFaduhv9rQ9SF5XHKyeyOie6xcG5n7IeMTI890="/>
-    <hyperlink ref="F7" r:id="rId13" display="http://www.infineon.com/dgdl/Infineon-IPD30N06S2L_23-DS-v01_00-en.pdf?fileId=db3a304412b407950112b433bafe5d69"/>
-    <hyperlink ref="G7" r:id="rId14" display="https://www.digikey.com/product-detail/en/infineon-technologies/IPD30N06S2L23ATMA3/IPD30N06S2L23ATMA3CT-ND/5440904"/>
-    <hyperlink ref="H7" r:id="rId15" display="http://www.mouser.com/ProductDetail/Infineon-Technologies/IPD30N06S2L23ATMA3/?qs=nKAiUEXvm/A3t2VUC031Ag=="/>
-    <hyperlink ref="F8" r:id="rId16" display="http://www.fairchildsemi.com/datasheets/1N/1N4731A.pdf"/>
-    <hyperlink ref="G8" r:id="rId17" display="https://www.digikey.com/product-detail/en/fairchild-semiconductor/1N4749A_T50A/1N4749A_T50AFSCT-ND/3478158"/>
-    <hyperlink ref="H8" r:id="rId18" display="http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/1N4749A_T50A/?qs=9h%2BT/FFCxR/U89fjfSyrjQ=="/>
-    <hyperlink ref="F9" r:id="rId19" display="http://www.diodes.com/_files/datasheets/ds30217.pdf"/>
-    <hyperlink ref="G9" r:id="rId20" display="https://www.digikey.com/product-detail/en/diodes-incorporated/1N5819HW-7-F/1N5819HW-FDICT-ND/815283"/>
-    <hyperlink ref="H9" r:id="rId21" display="http://www.mouser.com/ProductDetail/Diodes-Incorporated/1N5819HW-7-F/?qs=NQ47qNm99eDyWTEd07miYA=="/>
-    <hyperlink ref="F10" r:id="rId22" display="https://media.digikey.com/pdf/Data Sheets/Osram PDFs/LB_LT Q39G.pdf"/>
-    <hyperlink ref="G10" r:id="rId23" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LB-Q39G-L2OO-35-1/475-2816-1-ND/2176355"/>
-    <hyperlink ref="H10" r:id="rId24" display="http://www.mouser.com/ProductDetail/Osram-Opto-Semiconductor/LB-Q39G-L2OO-35-1/?qs=/ha2pyFadugdwYCal9BdM9SWhVbJU5uqsKvsYGbR4IvEO9KLCpls7BBaJhTRZMg6"/>
-    <hyperlink ref="F11" r:id="rId25" display="http://www.seielect.com/catalog/SEI-CF_CFM.pdf"/>
-    <hyperlink ref="G11" r:id="rId26" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT100K/CF14JT100KCT-ND/1830399"/>
-    <hyperlink ref="H11" r:id="rId27" display="http://www.mouser.com/ProductDetail/Ohmite/OK1045E-R52/?qs=sGAEpiMZZMsPqMdJzcrNwhqiT%2B35FJji0CucJiszflQ="/>
-    <hyperlink ref="F12" r:id="rId28" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW"/>
-    <hyperlink ref="G12" r:id="rId29" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1000V/P100HCT-ND/198109"/>
-    <hyperlink ref="H12" r:id="rId30" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=/ha2pyFaduglTbPDDZSypXi%2B1JYi5TJRT2R7dib9ms/8H45gLlep/g=="/>
-    <hyperlink ref="F13" r:id="rId31" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1002V+7+WW"/>
-    <hyperlink ref="G13" r:id="rId32" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1002V/P10.0KHCT-ND/198102"/>
-    <hyperlink ref="H13" r:id="rId33" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1002V/?qs=H7k1u0Mp9JSrGPQ5/5COuw=="/>
-    <hyperlink ref="F14" r:id="rId34" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF2200V+7+WW"/>
-    <hyperlink ref="G14" r:id="rId35" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF2200V/P220HCT-ND/1746741"/>
-    <hyperlink ref="H14" r:id="rId36" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF2200V/?qs=iBwFsHVUAOcTUCNoJPNpnQ=="/>
-    <hyperlink ref="F15" r:id="rId37" display="http://www.belfuse.com/pdfs/0ZCJ.pdf"/>
-    <hyperlink ref="G15" r:id="rId38" display="https://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCJ0050AF2E/507-1803-1-ND/4156312"/>
-    <hyperlink ref="H15" r:id="rId39" display="http://www.mouser.com/ProductDetail/Bel-Fuse/0ZCJ0050AF2E/?qs=SRYZG9HaIQ3Oqm1PQp276Q=="/>
-    <hyperlink ref="F16" r:id="rId40" display="http://industrial.panasonic.com/cdbs/www-data/pdf/RDE0000/ABA0000C1184.pdf"/>
-    <hyperlink ref="G16" r:id="rId41" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEE-FPV680XAP/PCE4553CT-ND/1701052"/>
-    <hyperlink ref="H16" r:id="rId42" display="http://www.mouser.com/ProductDetail/Panasonic/EEE-FPV680XAP/?qs=d1CqaRUMZD%2BB3QneHdz%2BNA=="/>
-    <hyperlink ref="F17" r:id="rId43" display="http://datasheets.avx.com/tps.pdf"/>
-    <hyperlink ref="G17" r:id="rId44" display="https://www.digikey.com/product-detail/en/avx-corporation/TPSD107K016R0125/478-1778-1-ND/564810"/>
-    <hyperlink ref="H17" r:id="rId45" display="http://www.mouser.com/ProductDetail/AVX/TPSD107K016R0125/?qs=Ow%2BOiPmaljGaFh%2BHI/q%2BNg=="/>
-    <hyperlink ref="F19" r:id="rId46" display="http://productfinder.pulseeng.com/products/datasheets/SPM2007_47.pdf"/>
-    <hyperlink ref="G19" r:id="rId47" display="https://www.digikey.com/product-detail/en/pulse-electronics-corporation/PE-53820SNL/553-1403-ND/1037014"/>
-    <hyperlink ref="H19" r:id="rId48" display="http://www.mouser.com/ProductDetail/Pulse/PE-53820SNL/?qs=sGAEpiMZZMsg%2By3WlYCkU6/kcGZFUWykAerZ435ceU4="/>
-    <hyperlink ref="F20" r:id="rId49" display="https://media.digikey.com/pdf/Data Sheets/CW Industries PDFs/GF-123-0054_Dwg.pdf"/>
-    <hyperlink ref="G20" r:id="rId50" display="https://www.digikey.com/product-detail/en/cw-industries/GF-123-0054/CWI333-ND/4089770"/>
-    <hyperlink ref="H20" r:id="rId51" display="http://www.mouser.com/ProductDetail/CW-Industries/GF-123-0054/?qs=n1d6TrdN4SA9FY9ssLiRzw=="/>
-    <hyperlink ref="F21" r:id="rId52" display="https://media.digikey.com/pdf/Data Sheets/Phoenix Contact PDFs/1935174.pdf"/>
-    <hyperlink ref="G21" r:id="rId53" display="https://www.digikey.com/product-detail/en/phoenix-contact/1935174/277-1578-ND/568615"/>
-    <hyperlink ref="H21" r:id="rId54" display="http://www.mouser.com/ProductDetail/Phoenix-Contact/1935174/?qs=QWULklcAmSR8B7o4YouITA=="/>
-    <hyperlink ref="F22" r:id="rId55" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
-    <hyperlink ref="G22" r:id="rId56" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-103HLF/609-3461-ND/2023309"/>
-    <hyperlink ref="H22" r:id="rId57" display="http://www.mouser.com/ProductDetail/FCI/68000-103HLF/?qs=zh4O8xspOuyqPBhcuxtliw=="/>
+    <hyperlink ref="F6" r:id="rId10" display="http://www.diodes.com/_files/datasheets/AP7313.pdf"/>
+    <hyperlink ref="G6" r:id="rId11" display="https://www.digikey.com/product-detail/en/diodes-incorporated/AP7313-18SAG-7/AP7313-18SAG-7DICT-ND/2270838"/>
+    <hyperlink ref="H6" r:id="rId12" display="http://www.mouser.com/ProductDetail/Diodes-Incorporated/AP7313-18SAG-7/?qs=/ha2pyFadujy/gnw%2B3xItPhBQ0SnhtM987cdGDCE3x6s1BRWXYc%2B1Q=="/>
+    <hyperlink ref="F8" r:id="rId13" display="https://www.winbond.com/resource-files/w25q128fv_revhh1_100913_website1.pdf"/>
+    <hyperlink ref="G8" r:id="rId14" display="https://www.digikey.com/product-search/en/integrated-circuits-ics/memory/2556980?k=w25q128fv&amp;k=&amp;pkeyword=w25q128fv&amp;pv16=7409&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25"/>
+    <hyperlink ref="F10" r:id="rId15" display="http://www.mouser.com/ds/2/368/Bluegigga%20Technologies_WT32i_Datasheet-558681.pdf"/>
+    <hyperlink ref="G10" r:id="rId16" display="https://www.digikey.com/product-detail/en/silicon-labs/WT32I-E-AI6/1446-1037-1-ND/4806564"/>
+    <hyperlink ref="H10" r:id="rId17" display="http://www.mouser.com/ProductDetail/Silicon-Labs-Bluegiga/WT32i-E-AI6/?qs=sGAEpiMZZMs8jstQXqv0yeC3dKQ4sq/l%2BU8bwDMPAJ4="/>
+    <hyperlink ref="F11" r:id="rId18" display="https://www.fairchildsemi.com/datasheets/FQ/FQP47P06.pdf"/>
+    <hyperlink ref="G11" r:id="rId19" display="https://www.digikey.com/product-detail/en/fairchild-semiconductor/FQP47P06/FQP47P06-ND/1057079"/>
+    <hyperlink ref="H11" r:id="rId20" display="http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/FQP47P06/?qs=/ha2pyFaduhv9rQ9SF5XHKyeyOie6xcG5n7IeMTI890="/>
+    <hyperlink ref="F12" r:id="rId21" display="http://www.infineon.com/dgdl/Infineon-IPD30N06S2L_23-DS-v01_00-en.pdf?fileId=db3a304412b407950112b433bafe5d69"/>
+    <hyperlink ref="G12" r:id="rId22" display="https://www.digikey.com/product-detail/en/infineon-technologies/IPD30N06S2L23ATMA3/IPD30N06S2L23ATMA3CT-ND/5440904"/>
+    <hyperlink ref="H12" r:id="rId23" display="http://www.mouser.com/ProductDetail/Infineon-Technologies/IPD30N06S2L23ATMA3/?qs=nKAiUEXvm/A3t2VUC031Ag=="/>
+    <hyperlink ref="F13" r:id="rId24" display="http://www.fairchildsemi.com/datasheets/1N/1N4731A.pdf"/>
+    <hyperlink ref="G13" r:id="rId25" display="https://www.digikey.com/product-detail/en/fairchild-semiconductor/1N4749A_T50A/1N4749A_T50AFSCT-ND/3478158"/>
+    <hyperlink ref="H13" r:id="rId26" display="http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/1N4749A_T50A/?qs=9h%2BT/FFCxR/U89fjfSyrjQ=="/>
+    <hyperlink ref="F14" r:id="rId27" display="http://www.diodes.com/_files/datasheets/ds30217.pdf"/>
+    <hyperlink ref="G14" r:id="rId28" display="https://www.digikey.com/product-detail/en/diodes-incorporated/1N5819HW-7-F/1N5819HW-FDICT-ND/815283"/>
+    <hyperlink ref="H14" r:id="rId29" display="http://www.mouser.com/ProductDetail/Diodes-Incorporated/1N5819HW-7-F/?qs=NQ47qNm99eDyWTEd07miYA=="/>
+    <hyperlink ref="F15" r:id="rId30" display="http://www.osram-os.com/Graphics/XPic2/00077107_0.pdf"/>
+    <hyperlink ref="G15" r:id="rId31" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LG-L29K-G2J1-24-Z/475-2709-1-ND/1938876"/>
+    <hyperlink ref="H15" r:id="rId32" display="http://www.mouser.com/ProductDetail/Osram-Opto-Semiconductor/LG-L29K-G2J1-24-Z/?qs=/ha2pyFadujpFotHoYnHK8u84Sh%2BBbQboBL3gK2afekn5czm8naaMg=="/>
+    <hyperlink ref="F16" r:id="rId33" display="https://media.digikey.com/pdf/Data Sheets/Osram PDFs/LB_LT Q39G.pdf"/>
+    <hyperlink ref="G16" r:id="rId34" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LB-Q39G-L2OO-35-1/475-2816-1-ND/2176355"/>
+    <hyperlink ref="H16" r:id="rId35" display="http://www.mouser.com/ProductDetail/Osram-Opto-Semiconductor/LB-Q39G-L2OO-35-1/?qs=/ha2pyFadugdwYCal9BdM9SWhVbJU5uqsKvsYGbR4IvEO9KLCpls7BBaJhTRZMg6"/>
+    <hyperlink ref="F17" r:id="rId36" display="http://www.seielect.com/catalog/SEI-CF_CFM.pdf"/>
+    <hyperlink ref="G17" r:id="rId37" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT100K/CF14JT100KCT-ND/1830399"/>
+    <hyperlink ref="H17" r:id="rId38" display="http://www.mouser.com/ProductDetail/Ohmite/OK1045E-R52/?qs=sGAEpiMZZMsPqMdJzcrNwhqiT%2B35FJji0CucJiszflQ="/>
+    <hyperlink ref="F18" r:id="rId39" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF8200V+7+WW"/>
+    <hyperlink ref="G18" r:id="rId40" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF8200V/P820HCT-ND/1746806"/>
+    <hyperlink ref="H18" r:id="rId41" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF8200V/?qs=/ha2pyFaduglTbPDDZSypYYGUgtAbfv2yF2HHUYX9QFp3giBobQZgg=="/>
+    <hyperlink ref="F19" r:id="rId42" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW"/>
+    <hyperlink ref="G19" r:id="rId43" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1000V/P100HCT-ND/198109"/>
+    <hyperlink ref="H19" r:id="rId44" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=H7k1u0Mp9JS7i8KGO5m47A=="/>
+    <hyperlink ref="F20" r:id="rId45" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1002V+7+WW"/>
+    <hyperlink ref="G20" r:id="rId46" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1002V/P10.0KHCT-ND/198102"/>
+    <hyperlink ref="H20" r:id="rId47" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1002V/?qs=H7k1u0Mp9JSrGPQ5/5COuw=="/>
+    <hyperlink ref="F21" r:id="rId48" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF2200V+7+WW"/>
+    <hyperlink ref="G21" r:id="rId49" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF2200V/P220HCT-ND/1746741"/>
+    <hyperlink ref="H21" r:id="rId50" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF2200V/?qs=iBwFsHVUAOcTUCNoJPNpnQ=="/>
+    <hyperlink ref="F23" r:id="rId51" display="http://www.belfuse.com/pdfs/0ZCJ.pdf"/>
+    <hyperlink ref="G23" r:id="rId52" display="https://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCJ0050AF2E/507-1803-1-ND/4156312"/>
+    <hyperlink ref="H23" r:id="rId53" display="http://www.mouser.com/ProductDetail/Bel-Fuse/0ZCJ0050AF2E/?qs=SRYZG9HaIQ3Oqm1PQp276Q=="/>
+    <hyperlink ref="F24" r:id="rId54" display="http://industrial.panasonic.com/cdbs/www-data/pdf/RDE0000/ABA0000C1184.pdf"/>
+    <hyperlink ref="G24" r:id="rId55" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEE-FPV680XAP/PCE4553CT-ND/1701052"/>
+    <hyperlink ref="H24" r:id="rId56" display="http://www.mouser.com/ProductDetail/Panasonic/EEE-FPV680XAP/?qs=d1CqaRUMZD%2BB3QneHdz%2BNA=="/>
+    <hyperlink ref="F25" r:id="rId57" display="http://datasheets.avx.com/tps.pdf"/>
+    <hyperlink ref="G25" r:id="rId58" display="https://www.digikey.com/product-detail/en/avx-corporation/TPSD107K016R0125/478-1778-1-ND/564810"/>
+    <hyperlink ref="H25" r:id="rId59" display="http://www.mouser.com/ProductDetail/AVX/TPSD107K016R0125/?qs=Ow%2BOiPmaljGaFh%2BHI/q%2BNg=="/>
+    <hyperlink ref="F29" r:id="rId60" display="http://productfinder.pulseeng.com/products/datasheets/SPM2007_47.pdf"/>
+    <hyperlink ref="G29" r:id="rId61" display="https://www.digikey.com/product-detail/en/pulse-electronics-corporation/PE-53820SNL/553-1403-ND/1037014"/>
+    <hyperlink ref="H29" r:id="rId62" display="http://www.mouser.com/ProductDetail/Pulse/PE-53820SNL/?qs=sGAEpiMZZMsg%2By3WlYCkU6/kcGZFUWykAerZ435ceU4="/>
+    <hyperlink ref="F30" r:id="rId63" display="https://product.tdk.com/info/en/catalog/datasheets/beads_commercial_power_mpz1608_en.pdf"/>
+    <hyperlink ref="G30" r:id="rId64" display="https://www.digikey.com/product-detail/en/tdk-corporation/MPZ1608S601ATA00/445-2205-1-ND/765103"/>
+    <hyperlink ref="H30" r:id="rId65" display="http://www.mouser.com/ProductDetail/TDK/MPZ1608S601ATA00/?qs=47dIwT2ZIzth0CTKDYh9rw=="/>
+    <hyperlink ref="F31" r:id="rId66" display="https://media.digikey.com/pdf/Data Sheets/CW Industries PDFs/GF-123-0054_Dwg.pdf"/>
+    <hyperlink ref="G31" r:id="rId67" display="https://www.digikey.com/product-detail/en/cw-industries/GF-123-0054/CWI333-ND/4089770"/>
+    <hyperlink ref="H31" r:id="rId68" display="http://www.mouser.com/ProductDetail/CW-Industries/GF-123-0054/?qs=n1d6TrdN4SA9FY9ssLiRzw=="/>
+    <hyperlink ref="F33" r:id="rId69" display="https://media.digikey.com/pdf/Data Sheets/Phoenix Contact PDFs/1935174.pdf"/>
+    <hyperlink ref="G33" r:id="rId70" display="https://www.digikey.com/product-detail/en/phoenix-contact/1935174/277-1578-ND/568615"/>
+    <hyperlink ref="H33" r:id="rId71" display="http://www.mouser.com/ProductDetail/Phoenix-Contact/1935174/?qs=QWULklcAmSR8B7o4YouITA=="/>
+    <hyperlink ref="F34" r:id="rId72" display="http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf"/>
+    <hyperlink ref="G34" r:id="rId73" display="https://www.digikey.com/product-detail/en/amphenol-fci/68000-103HLF/609-3461-ND/2023309"/>
+    <hyperlink ref="H34" r:id="rId74" display="http://www.mouser.com/ProductDetail/FCI/68000-103HLF/?qs=zh4O8xspOuyqPBhcuxtliw=="/>
+    <hyperlink ref="F36" r:id="rId75" display="http://www.digi.com/products/models/jf1r6-cr3-4i"/>
+    <hyperlink ref="G36" r:id="rId76" display="https://www.digikey.com/product-detail/en/digi-international/JF1R6-CR3-4I/JF1R6-CR3-4I-ND/1090366"/>
+    <hyperlink ref="H36" r:id="rId77" display="http://www.mouser.com/ProductDetail/Digi-International/JF1R6-CR3-4I/?qs=/ha2pyFaduims8tK6Us52r5eWOHgAet92us06mmlXyAvpYrNpBxg1A=="/>
+    <hyperlink ref="F37" r:id="rId78" display="http://www.lsr.com/downloads/products/330-0150.pdf"/>
+    <hyperlink ref="G37" r:id="rId79" display="https://www.digikey.com/product-detail/en/lsr/001-0015/001-0015-ND/4732759"/>
+    <hyperlink ref="H37" r:id="rId80" display="http://www.mouser.com/ProductDetail/LS-Research/001-0015/?qs=sGAEpiMZZMuBTKBKvsBmlP%2BmDojcpAG/Vyhv39d/eWhHn2QU78Oagg=="/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.02638888888889" bottom="1.02638888888889" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>